<commit_message>
update buoyancy flux metadata
</commit_message>
<xml_diff>
--- a/meta-data/flux-estimates-level1.xlsx
+++ b/meta-data/flux-estimates-level1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/AOM-WP1-BL/meta-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5FD85A-9E3E-6A4E-A2F1-D1FE26D59A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD2D1B0-C527-9A4D-A690-FCD4746FEEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="6260" windowWidth="28800" windowHeight="18220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="2220" windowWidth="15700" windowHeight="18220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="variables-specific" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="91">
   <si>
     <t>Variable</t>
   </si>
@@ -106,9 +106,6 @@
     <t>buoyancy_flux</t>
   </si>
   <si>
-    <t>J m-2 s-1</t>
-  </si>
-  <si>
     <t>cell_methods</t>
   </si>
   <si>
@@ -256,9 +253,6 @@
     <t>&lt;derived from file&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Buoyancy Flux (&lt;w'Ts'&gt;) </t>
-  </si>
-  <si>
     <t>time: mean</t>
   </si>
   <si>
@@ -296,6 +290,9 @@
   </si>
   <si>
     <t>Quality flag: WQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buoyancy Flux (&lt;w'Ts'&gt;*rho*Cp) </t>
   </si>
 </sst>
 </file>
@@ -732,8 +729,8 @@
   </sheetPr>
   <dimension ref="A1:F968"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
-      <selection activeCell="C260" sqref="C260"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -819,7 +816,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -827,7 +824,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -893,7 +890,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -901,7 +898,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -915,7 +912,7 @@
     <row r="21" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="22" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -939,7 +936,7 @@
         <v>3</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -947,7 +944,7 @@
         <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -963,7 +960,7 @@
         <v>17</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D28" s="4"/>
     </row>
@@ -972,15 +969,15 @@
         <v>18</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1045,7 +1042,7 @@
         <v>17</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D39" s="4"/>
     </row>
@@ -1054,7 +1051,7 @@
         <v>18</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1095,7 +1092,7 @@
         <v>3</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1103,7 +1100,7 @@
         <v>14</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1119,7 +1116,7 @@
         <v>17</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1127,15 +1124,15 @@
         <v>18</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B51" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="D51" s="4"/>
     </row>
@@ -1152,7 +1149,7 @@
     </row>
     <row r="54" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C54" s="4"/>
     </row>
@@ -1177,7 +1174,7 @@
         <v>3</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1185,7 +1182,7 @@
         <v>14</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1201,7 +1198,7 @@
         <v>17</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1209,16 +1206,16 @@
         <v>18</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D61" s="4"/>
     </row>
     <row r="62" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B62" t="s">
+        <v>28</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1234,7 +1231,7 @@
     </row>
     <row r="65" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C65" s="4"/>
     </row>
@@ -1259,7 +1256,7 @@
         <v>3</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1267,7 +1264,7 @@
         <v>14</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1283,7 +1280,7 @@
         <v>17</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1291,15 +1288,15 @@
         <v>18</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B73" t="s">
+        <v>28</v>
+      </c>
+      <c r="C73" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1315,7 +1312,7 @@
     </row>
     <row r="76" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C76" s="4"/>
     </row>
@@ -1340,7 +1337,7 @@
         <v>3</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1348,7 +1345,7 @@
         <v>14</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1364,7 +1361,7 @@
         <v>17</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1372,15 +1369,15 @@
         <v>18</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B84" t="s">
+        <v>28</v>
+      </c>
+      <c r="C84" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1396,7 +1393,7 @@
     </row>
     <row r="87" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C87" s="4"/>
     </row>
@@ -1421,7 +1418,7 @@
         <v>3</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1429,7 +1426,7 @@
         <v>13</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1437,7 +1434,7 @@
         <v>14</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1453,7 +1450,7 @@
         <v>17</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1461,15 +1458,15 @@
         <v>18</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B96" t="s">
+        <v>28</v>
+      </c>
+      <c r="C96" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C96" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1486,7 +1483,7 @@
     </row>
     <row r="99" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A99" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C99" s="4"/>
     </row>
@@ -1511,7 +1508,7 @@
         <v>3</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1519,7 +1516,7 @@
         <v>13</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1527,7 +1524,7 @@
         <v>14</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1543,7 +1540,7 @@
         <v>17</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1551,15 +1548,15 @@
         <v>18</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B108" t="s">
+        <v>28</v>
+      </c>
+      <c r="C108" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C108" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1576,7 +1573,7 @@
     </row>
     <row r="111" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A111" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C111" s="4"/>
     </row>
@@ -1601,7 +1598,7 @@
         <v>3</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1609,7 +1606,7 @@
         <v>14</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1625,7 +1622,7 @@
         <v>17</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1633,15 +1630,15 @@
         <v>18</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B119" t="s">
+        <v>28</v>
+      </c>
+      <c r="C119" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C119" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1657,7 +1654,7 @@
     </row>
     <row r="122" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A122" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C122" s="4"/>
       <c r="D122" s="4"/>
@@ -1683,7 +1680,7 @@
         <v>3</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1691,7 +1688,7 @@
         <v>14</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1707,7 +1704,7 @@
         <v>17</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1715,15 +1712,15 @@
         <v>18</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B130" t="s">
+        <v>28</v>
+      </c>
+      <c r="C130" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C130" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1739,7 +1736,7 @@
     </row>
     <row r="133" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A133" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C133" s="4"/>
     </row>
@@ -1772,7 +1769,7 @@
         <v>14</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1788,7 +1785,7 @@
         <v>17</v>
       </c>
       <c r="C139" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1796,15 +1793,15 @@
         <v>18</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B141" t="s">
+        <v>28</v>
+      </c>
+      <c r="C141" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C141" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1820,7 +1817,7 @@
     </row>
     <row r="144" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A144" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B144" s="9"/>
       <c r="C144" s="4"/>
@@ -1831,7 +1828,7 @@
         <v>8</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1858,25 +1855,25 @@
         <v>14</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A149" s="9"/>
       <c r="B149" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C149" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A150" s="9"/>
       <c r="B150" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C150" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1884,7 +1881,7 @@
     </row>
     <row r="152" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A152" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B152" s="9"/>
       <c r="C152" s="4"/>
@@ -1895,7 +1892,7 @@
         <v>8</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1922,25 +1919,25 @@
         <v>14</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A157" s="9"/>
       <c r="B157" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C157" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A158" s="9"/>
       <c r="B158" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C158" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1950,7 +1947,7 @@
     </row>
     <row r="160" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A160" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B160" s="9"/>
       <c r="C160" s="4"/>
@@ -1961,7 +1958,7 @@
         <v>8</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1988,25 +1985,25 @@
         <v>14</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A165" s="9"/>
       <c r="B165" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C165" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A166" s="9"/>
       <c r="B166" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C166" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="167" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2016,7 +2013,7 @@
     </row>
     <row r="168" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A168" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B168" s="9"/>
       <c r="C168" s="4"/>
@@ -2027,7 +2024,7 @@
         <v>8</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2054,25 +2051,25 @@
         <v>14</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A173" s="9"/>
       <c r="B173" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C173" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A174" s="9"/>
       <c r="B174" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C174" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="175" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2082,7 +2079,7 @@
     </row>
     <row r="176" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A176" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B176" s="9"/>
       <c r="C176" s="4"/>
@@ -2093,7 +2090,7 @@
         <v>8</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2120,25 +2117,25 @@
         <v>14</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A181" s="9"/>
       <c r="B181" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C181" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A182" s="9"/>
       <c r="B182" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C182" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2148,7 +2145,7 @@
     </row>
     <row r="184" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A184" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B184" s="9"/>
       <c r="C184" s="4"/>
@@ -2159,7 +2156,7 @@
         <v>8</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2186,25 +2183,25 @@
         <v>14</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A189" s="9"/>
       <c r="B189" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C189" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A190" s="9"/>
       <c r="B190" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C190" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2214,7 +2211,7 @@
     </row>
     <row r="192" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A192" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B192" s="9"/>
       <c r="C192" s="4"/>
@@ -2225,7 +2222,7 @@
         <v>8</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="194" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2252,25 +2249,25 @@
         <v>14</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="197" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A197" s="9"/>
       <c r="B197" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C197" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="198" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A198" s="9"/>
       <c r="B198" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C198" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="199" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2280,7 +2277,7 @@
     </row>
     <row r="200" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A200" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B200" s="9"/>
       <c r="C200" s="4"/>
@@ -2291,7 +2288,7 @@
         <v>8</v>
       </c>
       <c r="C201" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2318,25 +2315,25 @@
         <v>14</v>
       </c>
       <c r="C204" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="205" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A205" s="9"/>
       <c r="B205" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C205" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="206" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A206" s="9"/>
       <c r="B206" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C206" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="207" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2346,7 +2343,7 @@
     </row>
     <row r="208" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A208" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B208" s="9"/>
       <c r="C208" s="4"/>
@@ -2357,7 +2354,7 @@
         <v>8</v>
       </c>
       <c r="C209" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="210" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2384,25 +2381,25 @@
         <v>14</v>
       </c>
       <c r="C212" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="213" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A213" s="9"/>
       <c r="B213" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C213" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="214" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A214" s="9"/>
       <c r="B214" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C214" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2412,7 +2409,7 @@
     </row>
     <row r="216" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A216" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B216" s="9"/>
       <c r="C216" s="4"/>
@@ -2423,7 +2420,7 @@
         <v>8</v>
       </c>
       <c r="C217" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="218" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2450,25 +2447,25 @@
         <v>14</v>
       </c>
       <c r="C220" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="221" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A221" s="9"/>
       <c r="B221" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C221" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="222" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A222" s="9"/>
       <c r="B222" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C222" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="223" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2478,7 +2475,7 @@
     </row>
     <row r="224" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A224" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B224" s="9"/>
       <c r="C224" s="4"/>
@@ -2489,7 +2486,7 @@
         <v>8</v>
       </c>
       <c r="C225" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="226" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2516,25 +2513,25 @@
         <v>14</v>
       </c>
       <c r="C228" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="229" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A229" s="9"/>
       <c r="B229" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C229" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A230" s="9"/>
       <c r="B230" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C230" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="231" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2544,7 +2541,7 @@
     </row>
     <row r="232" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A232" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B232" s="9"/>
       <c r="C232" s="4"/>
@@ -2555,7 +2552,7 @@
         <v>8</v>
       </c>
       <c r="C233" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="234" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2582,25 +2579,25 @@
         <v>14</v>
       </c>
       <c r="C236" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="237" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A237" s="9"/>
       <c r="B237" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C237" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="238" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A238" s="9"/>
       <c r="B238" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C238" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="239" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2610,7 +2607,7 @@
     </row>
     <row r="240" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A240" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B240" s="9"/>
       <c r="C240" s="4"/>
@@ -2621,7 +2618,7 @@
         <v>8</v>
       </c>
       <c r="C241" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="242" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2648,25 +2645,25 @@
         <v>14</v>
       </c>
       <c r="C244" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="245" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A245" s="9"/>
       <c r="B245" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C245" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="246" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A246" s="9"/>
       <c r="B246" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C246" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="247" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2676,7 +2673,7 @@
     </row>
     <row r="248" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A248" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B248" s="9"/>
       <c r="C248" s="4"/>
@@ -2687,7 +2684,7 @@
         <v>8</v>
       </c>
       <c r="C249" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="250" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -2714,25 +2711,25 @@
         <v>14</v>
       </c>
       <c r="C252" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="253" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A253" s="9"/>
       <c r="B253" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C253" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="254" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A254" s="9"/>
       <c r="B254" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C254" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="255" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>